<commit_message>
do not try to estimate beta
</commit_message>
<xml_diff>
--- a/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
+++ b/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11685" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>beta</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>gamma</t>
   </si>
@@ -397,7 +394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -405,7 +402,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -5418,15 +5415,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5439,11 +5436,8 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5456,15 +5450,9 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="D3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
do not try to estimate gamma either
</commit_message>
<xml_diff>
--- a/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
+++ b/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>gamma</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>gBar</t>
   </si>
@@ -402,7 +399,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -5415,15 +5412,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5433,11 +5430,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5447,12 +5441,9 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "do not try to estimate gamma either"
This reverts commit 824d7c8cd01108e08acf5797264fce86ec948e7e.
</commit_message>
<xml_diff>
--- a/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
+++ b/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
@@ -25,7 +25,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>gamma</t>
+  </si>
   <si>
     <t>gBar</t>
   </si>
@@ -399,7 +402,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -5412,15 +5415,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5430,8 +5433,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5441,9 +5447,12 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "do not try to estimate beta"
This reverts commit 080599df5cda0fcd6871dc5bd4e056f3e7d6bec0.
</commit_message>
<xml_diff>
--- a/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
+++ b/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11685" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11685"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>beta</t>
+  </si>
   <si>
     <t>gamma</t>
   </si>
@@ -394,7 +397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -402,7 +405,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -5415,15 +5418,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5436,8 +5439,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5450,9 +5456,15 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
explicit upper bounds on beta and rho below 1
</commit_message>
<xml_diff>
--- a/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
+++ b/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11685" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -5420,8 +5420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5462,10 +5462,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>0.99999899999999997</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0.99999899999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
place a lower bound on beta too
</commit_message>
<xml_diff>
--- a/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
+++ b/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
@@ -5421,7 +5421,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5445,7 +5445,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="B2">
         <v>0</v>

</xml_diff>

<commit_message>
never estimate gamma, and don't estimate beta without bounds
</commit_message>
<xml_diff>
--- a/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
+++ b/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11685" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>beta</t>
-  </si>
-  <si>
-    <t>gamma</t>
   </si>
   <si>
     <t>gBar</t>
@@ -397,7 +394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A1001"/>
     </sheetView>
   </sheetViews>
@@ -405,7 +402,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -5418,15 +5415,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5439,11 +5436,8 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9.9999999999999995E-7</v>
       </c>
@@ -5456,15 +5450,12 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.99999899999999997</v>
       </c>
-      <c r="D3">
+      <c r="C3">
         <v>0.99999899999999997</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lower bound on gbar
</commit_message>
<xml_diff>
--- a/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
+++ b/Examples/BoundedProductivityEstimation/BoundedProductivityEstimation.xlsx
@@ -5418,7 +5418,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5442,7 +5442,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="C2">
         <v>0</v>

</xml_diff>